<commit_message>
More exp 2 analysis updates
</commit_message>
<xml_diff>
--- a/Production-Casemarking/Analysis - Post Blindcoding/1graphs for thesis.xlsx
+++ b/Production-Casemarking/Analysis - Post Blindcoding/1graphs for thesis.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="15460" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="12260" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Graph 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Graph 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Graph 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Graph 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Graph 5" sheetId="5" r:id="rId5"/>
-    <sheet name="Graph 6" sheetId="6" r:id="rId6"/>
-    <sheet name="Graph 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Graph 3" sheetId="3" r:id="rId2"/>
+    <sheet name="Graph 5" sheetId="5" r:id="rId3"/>
+    <sheet name="Graph 2" sheetId="2" r:id="rId4"/>
+    <sheet name="Graph 6" sheetId="6" r:id="rId5"/>
+    <sheet name="Graph 7" sheetId="7" r:id="rId6"/>
+    <sheet name="Graph 4" sheetId="4" r:id="rId7"/>
     <sheet name="Graph 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="105">
   <si>
     <t xml:space="preserve">            Case      Free</t>
   </si>
@@ -275,6 +275,72 @@
   </si>
   <si>
     <t>TRUE  0.6589599 0.2782430</t>
+  </si>
+  <si>
+    <t>FIGURE 4 in the paper</t>
+  </si>
+  <si>
+    <t>FIGURE 5</t>
+  </si>
+  <si>
+    <t>FIGURE 6</t>
+  </si>
+  <si>
+    <t>FIGURE 7</t>
+  </si>
+  <si>
+    <t>FIGURE 8</t>
+  </si>
+  <si>
+    <t>FIGURE 9</t>
+  </si>
+  <si>
+    <t>Task 1-No instruction</t>
+  </si>
+  <si>
+    <t>Task 2 - Casemarking instruction</t>
+  </si>
+  <si>
+    <t>Task 1 - No instruction</t>
+  </si>
+  <si>
+    <t>&gt; PersonFree.boot.mean = bootstrap(AnimacySpatialScores[AnimacySpatialScores$Object.Type=="Person" &amp; AnimacySpatialScores$GestureCondition=="Free",]$Casemarked, 1000, mean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1317645 0.3587032 </t>
+  </si>
+  <si>
+    <t>&gt; PersonHand.boot.mean = bootstrap(AnimacySpatialScores[AnimacySpatialScores$Object.Type=="Person" &amp; AnimacySpatialScores$GestureCondition=="Case",]$Casemarked, 1000, mean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8299320 0.9732993 </t>
+  </si>
+  <si>
+    <t>&gt; ObjectFree.boot.mean = bootstrap(AnimacySpatialScores[AnimacySpatialScores$Object.Type=="Object" &amp; AnimacySpatialScores$GestureCondition=="Free",]$Casemarked, 1000, mean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1799676 0.4219905 </t>
+  </si>
+  <si>
+    <t>&gt; ObjectHand.boot.mean = bootstrap(AnimacySpatialScores[AnimacySpatialScores$Object.Type=="Object" &amp; AnimacySpatialScores$GestureCondition=="Case",]$Casemarked, 1000, mean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7693793 0.9496599 </t>
+  </si>
+  <si>
+    <t>BootCI</t>
+  </si>
+  <si>
+    <t>&gt; PersonFree.boot.mean = bootstrap(EmbodPVScores[EmbodPVScores$Object.Type=="Person" &amp; EmbodPVScores$GestureCondition=="Free",]$PV.Embod, 1000, mean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5270196 0.7761930 </t>
+  </si>
+  <si>
+    <t>&gt; PersonHand.boot.mean = bootstrap(EmbodPVScores[EmbodPVScores$Object.Type=="Person" &amp; EmbodPVScores$GestureCondition=="Case",]$PV.Embod, 1000, mean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1953571 0.4294260 </t>
   </si>
 </sst>
 </file>
@@ -330,8 +396,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -384,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -408,6 +480,9 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -431,6 +506,9 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -523,10 +601,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>No instruction</c:v>
+                  <c:v>Task 1-No instruction</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Casemarking instruction</c:v>
+                  <c:v>Task 2 - Casemarking instruction</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -612,10 +690,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>No instruction</c:v>
+                  <c:v>Task 1-No instruction</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Casemarking instruction</c:v>
+                  <c:v>Task 2 - Casemarking instruction</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -645,11 +723,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2037582936"/>
-        <c:axId val="2085647464"/>
+        <c:axId val="2083086696"/>
+        <c:axId val="2094762472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2037582936"/>
+        <c:axId val="2083086696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -658,7 +736,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085647464"/>
+        <c:crossAx val="2094762472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -666,7 +744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2085647464"/>
+        <c:axId val="2094762472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -697,7 +775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2037582936"/>
+        <c:crossAx val="2083086696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -731,10 +809,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="122"/>
+      <c14:style val="120"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="22"/>
+      <c:style val="20"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -750,49 +828,84 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 2'!$A$29</c:f>
+              <c:f>'Graph 3'!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>No spatial cueing used</c:v>
+                  <c:v>Inanimate patient</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4">
+              <a:schemeClr val="accent2">
                 <a:lumMod val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Graph 3'!$B$33:$C$33</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.12</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.09</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Graph 3'!$B$33:$C$33</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.12</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.09</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 2'!$B$28:$C$28</c:f>
+              <c:f>'Graph 3'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>No instruction</c:v>
+                  <c:v>Task 1 - No instruction</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Casemarking instruction</c:v>
+                  <c:v>Task 2 - Casemarking instruction</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 2'!$B$29:$C$29</c:f>
+              <c:f>'Graph 3'!$B$29:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.414</c:v>
+                  <c:v>0.295</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -803,18 +916,18 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 2'!$A$30</c:f>
+              <c:f>'Graph 3'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Spatial cueing used</c:v>
+                  <c:v>Animate patient</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4">
+              <a:schemeClr val="accent2">
                 <a:lumMod val="60000"/>
                 <a:lumOff val="40000"/>
               </a:schemeClr>
@@ -822,31 +935,66 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Graph 3'!$B$34:$C$34</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.115</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.07</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Graph 3'!$B$34:$C$34</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.115</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.07</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 2'!$B$28:$C$28</c:f>
+              <c:f>'Graph 3'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>No instruction</c:v>
+                  <c:v>Task 1 - No instruction</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Casemarking instruction</c:v>
+                  <c:v>Task 2 - Casemarking instruction</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 2'!$B$30:$C$30</c:f>
+              <c:f>'Graph 3'!$B$30:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.847</c:v>
+                  <c:v>0.244</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.863</c:v>
+                  <c:v>0.912</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,11 +1009,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2110566072"/>
-        <c:axId val="2112522408"/>
+        <c:axId val="2096244872"/>
+        <c:axId val="2096247848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2110566072"/>
+        <c:axId val="2096244872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +1022,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112522408"/>
+        <c:crossAx val="2096247848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -882,9 +1030,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2112522408"/>
+        <c:axId val="2096247848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -900,8 +1049,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Proportion VNM orders (inc. SOV)</a:t>
+                  <a:t>Proportion</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of trials</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -912,7 +1066,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110566072"/>
+        <c:crossAx val="2096244872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -965,7 +1119,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 3'!$A$29</c:f>
+              <c:f>'Graph 5'!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -976,16 +1130,13 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
-            <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 3'!$B$28:$C$28</c:f>
+              <c:f>'Graph 5'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -999,15 +1150,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 3'!$B$29:$C$29</c:f>
+              <c:f>'Graph 5'!$B$29:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.295</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.866</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1018,7 +1169,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 3'!$A$30</c:f>
+              <c:f>'Graph 5'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1037,9 +1188,44 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Graph 5'!$B$34:$C$34</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.125</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.115</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Graph 5'!$B$34:$C$34</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.125</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.115</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 3'!$B$28:$C$28</c:f>
+              <c:f>'Graph 5'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1053,15 +1239,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 3'!$B$30:$C$30</c:f>
+              <c:f>'Graph 5'!$B$30:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.244</c:v>
+                  <c:v>0.654</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.912</c:v>
+                  <c:v>0.308</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,11 +1262,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2038646136"/>
-        <c:axId val="2109189896"/>
+        <c:axId val="2063456456"/>
+        <c:axId val="2063541768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2038646136"/>
+        <c:axId val="2063456456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1089,7 +1275,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109189896"/>
+        <c:crossAx val="2063541768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1097,9 +1283,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2109189896"/>
+        <c:axId val="2063541768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1115,13 +1302,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Proportion</a:t>
+                  <a:t>Proprtion of trials</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> trials with Casemarking/Spatial Cueing gestures</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1132,7 +1314,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2038646136"/>
+        <c:crossAx val="2063456456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1185,7 +1367,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 4'!$A$29</c:f>
+              <c:f>'Graph 2'!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1205,7 +1387,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 4'!$B$28:$C$28</c:f>
+              <c:f>'Graph 2'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1219,15 +1401,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 4'!$B$29:$C$29</c:f>
+              <c:f>'Graph 2'!$B$29:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.282</c:v>
+                  <c:v>0.414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.512</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1238,7 +1420,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 4'!$A$30</c:f>
+              <c:f>'Graph 2'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1259,7 +1441,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 4'!$B$28:$C$28</c:f>
+              <c:f>'Graph 2'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1273,15 +1455,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 4'!$B$30:$C$30</c:f>
+              <c:f>'Graph 2'!$B$30:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.819</c:v>
+                  <c:v>0.847</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.849</c:v>
+                  <c:v>0.863</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1296,11 +1478,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2091284296"/>
-        <c:axId val="2091790312"/>
+        <c:axId val="2092035080"/>
+        <c:axId val="2083101784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2091284296"/>
+        <c:axId val="2092035080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1491,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091790312"/>
+        <c:crossAx val="2083101784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1499,222 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091790312"/>
+        <c:axId val="2083101784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Proportion VNM orders (inc. SOV)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2092035080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="122"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="22"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph 6'!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Role conflict potential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graph 6'!$B$28:$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No instruction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Casemarking instruction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graph 6'!$B$29:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.279</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.626</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph 6'!$A$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No role conflict potential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graph 6'!$B$28:$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No instruction</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Casemarking instruction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graph 6'!$B$30:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.576</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.851</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2062780312"/>
+        <c:axId val="2096496248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2062780312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2096496248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2096496248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1354,227 +1751,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091284296"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Graph 5'!$A$29</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Inanimate patient</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Graph 5'!$B$28:$C$28</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>No instruction</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Casemarking instruction</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Graph 5'!$B$29:$C$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Graph 5'!$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Animate patient</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Graph 5'!$B$28:$C$28</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>No instruction</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Casemarking instruction</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Graph 5'!$B$30:$C$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.654</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.308</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2111020888"/>
-        <c:axId val="2095415576"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2111020888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095415576"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2095415576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Proprtion</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of trials with potential for role conflict (P,V body-based gesture)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111020888"/>
+        <c:crossAx val="2062780312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1608,6 +1785,227 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="117"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="17"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph 7'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Role conflict potential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graph 7'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No spatial cueing used</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spatial cueing used</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graph 7'!$B$13:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>149.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph 7'!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No role conflict potential</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graph 7'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>No spatial cueing used</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Spatial cueing used</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graph 7'!$B$14:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>205.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2096505736"/>
+        <c:axId val="2096626808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2096505736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2096626808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2096626808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>N. trials across both gesture tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2096505736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="122"/>
     </mc:Choice>
     <mc:Fallback>
@@ -1627,11 +2025,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 6'!$A$29</c:f>
+              <c:f>'Graph 4'!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Role conflict potential</c:v>
+                  <c:v>No spatial cueing used</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1647,7 +2045,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 6'!$B$28:$C$28</c:f>
+              <c:f>'Graph 4'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1661,15 +2059,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 6'!$B$29:$C$29</c:f>
+              <c:f>'Graph 4'!$B$29:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.279</c:v>
+                  <c:v>0.282</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.626</c:v>
+                  <c:v>0.512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,11 +2078,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graph 6'!$A$30</c:f>
+              <c:f>'Graph 4'!$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>No role conflict potential</c:v>
+                  <c:v>Spatial cueing used</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1701,7 +2099,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Graph 6'!$B$28:$C$28</c:f>
+              <c:f>'Graph 4'!$B$28:$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1715,15 +2113,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph 6'!$B$30:$C$30</c:f>
+              <c:f>'Graph 4'!$B$30:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.576</c:v>
+                  <c:v>0.819</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.851</c:v>
+                  <c:v>0.849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1738,11 +2136,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2090204808"/>
-        <c:axId val="2096075288"/>
+        <c:axId val="2096521992"/>
+        <c:axId val="2086338488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2090204808"/>
+        <c:axId val="2096521992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1751,7 +2149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2096075288"/>
+        <c:crossAx val="2086338488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1759,7 +2157,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2096075288"/>
+        <c:axId val="2086338488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1796,228 +2194,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090204808"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="117"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="17"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Graph 7'!$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Role conflict potential</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Graph 7'!$B$12:$C$12</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>No spatial cueing used</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Spatial cueing used</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Graph 7'!$B$13:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>149.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>93.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Graph 7'!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>No role conflict potential</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="65000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Graph 7'!$B$12:$C$12</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>No spatial cueing used</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Spatial cueing used</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Graph 7'!$B$14:$C$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>205.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2111722488"/>
-        <c:axId val="2111755800"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2111722488"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111755800"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2111755800"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>N. trials across both gesture tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111722488"/>
+        <c:crossAx val="2096521992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2181,11 +2358,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2113203656"/>
-        <c:axId val="2113206744"/>
+        <c:axId val="2083275608"/>
+        <c:axId val="2083278584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2113203656"/>
+        <c:axId val="2083275608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2194,7 +2371,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113206744"/>
+        <c:crossAx val="2083278584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2202,7 +2379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113206744"/>
+        <c:axId val="2083278584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2238,7 +2415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113203656"/>
+        <c:crossAx val="2083275608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2304,41 +2481,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>577850</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
       <xdr:row>19</xdr:row>
@@ -2370,42 +2512,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2440,7 +2547,42 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2475,7 +2617,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2489,6 +2631,41 @@
       <xdr:colOff>628650</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2867,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2998,10 +3175,10 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3126,6 +3303,11 @@
     <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7">
+      <c r="G51" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3142,252 +3324,202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B29">
-        <v>0.41399999999999998</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="C29">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>0.86599999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B30">
-        <v>0.84699999999999998</v>
+        <v>0.24399999999999999</v>
       </c>
       <c r="C30">
-        <v>0.86299999999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B33">
-        <v>0.29799999999999999</v>
+        <f>(0.42-0.18)/2</f>
+        <v>0.12</v>
       </c>
       <c r="C33">
-        <v>0.35</v>
-      </c>
-      <c r="E33" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33">
-        <f>(B37-B33)/2</f>
-        <v>0.12000000000000002</v>
-      </c>
-      <c r="G33">
-        <f>(C37-C33)/2</f>
-        <v>0.23749999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <f>(0.95-0.77)/2</f>
+        <v>8.9999999999999969E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B34">
-        <v>0.69099999999999995</v>
+        <f>(0.36-0.13)/2</f>
+        <v>0.11499999999999999</v>
       </c>
       <c r="C34">
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="E34" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34">
-        <f>(B38-B34)/2</f>
-        <v>0.13450000000000001</v>
-      </c>
-      <c r="G34">
-        <f>(C38-C34)/2</f>
-        <v>8.7499999999999967E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <f>(0.97-0.83)/2</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="H36" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37">
-        <v>0.53800000000000003</v>
-      </c>
-      <c r="C37">
-        <v>0.82499999999999996</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38">
-        <v>0.96</v>
-      </c>
-      <c r="C38">
-        <v>0.94299999999999995</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3404,50 +3536,85 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3457,31 +3624,70 @@
       <c r="C28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="H28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>22</v>
       </c>
       <c r="B29">
-        <v>0.29499999999999998</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>23</v>
       </c>
       <c r="B30">
-        <v>0.24399999999999999</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="C30">
-        <v>0.91200000000000003</v>
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <f>(0.78-0.53)/2</f>
+        <v>0.125</v>
+      </c>
+      <c r="C34">
+        <f>(0.43-0.2)/2</f>
+        <v>0.11499999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3493,40 +3699,120 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3537,26 +3823,133 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>47</v>
       </c>
       <c r="B29">
-        <v>0.28199999999999997</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="C29">
-        <v>0.51200000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>48</v>
       </c>
       <c r="B30">
-        <v>0.81899999999999995</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="C30">
-        <v>0.84899999999999998</v>
+        <v>0.86299999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="C33">
+        <v>0.35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33">
+        <f>(B37-B33)/2</f>
+        <v>0.12000000000000002</v>
+      </c>
+      <c r="G33">
+        <f>(C37-C33)/2</f>
+        <v>0.23749999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="C34">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34">
+        <f>(B38-B34)/2</f>
+        <v>0.13450000000000001</v>
+      </c>
+      <c r="G34">
+        <f>(C38-C34)/2</f>
+        <v>8.7499999999999967E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="C37">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38">
+        <v>0.96</v>
+      </c>
+      <c r="C38">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="K42" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3573,42 +3966,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>60</v>
+      <c r="A1" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -3624,28 +4017,34 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>0.626</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B30">
-        <v>0.65400000000000003</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="C30">
-        <v>0.308</v>
+        <v>0.85099999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="10:10">
+      <c r="J34" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3657,75 +4056,72 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B29">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="C29">
-        <v>0.626</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+      <c r="B13">
+        <v>149</v>
+      </c>
+      <c r="C13">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B30">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="C30">
-        <v>0.85099999999999998</v>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="8:8">
+      <c r="H24" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -3742,67 +4138,70 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>47</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B29">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="C29">
+        <v>0.51200000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13">
-        <v>149</v>
-      </c>
-      <c r="C13">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14">
-        <v>45</v>
-      </c>
-      <c r="C14">
-        <v>205</v>
+      <c r="B30">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="C30">
+        <v>0.84899999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>